<commit_message>
atualização da função de comprimentos
</commit_message>
<xml_diff>
--- a/data/safira_cana_planta.xlsx
+++ b/data/safira_cana_planta.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,6 +398,21 @@
           <t>comprimento</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>volume_cm3_dm3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>area_cm2_dm3</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>comprimento_cm_dm3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -432,6 +447,15 @@
       <c r="H2">
         <v>1267.04589706659</v>
       </c>
+      <c r="I2">
+        <v>3.351166849263158</v>
+      </c>
+      <c r="J2">
+        <v>90.74026724210526</v>
+      </c>
+      <c r="K2">
+        <v>266.7465046455979</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -466,6 +490,15 @@
       <c r="H3">
         <v>829.866975456476</v>
       </c>
+      <c r="I3">
+        <v>4.693151396147369</v>
+      </c>
+      <c r="J3">
+        <v>82.06963163368422</v>
+      </c>
+      <c r="K3">
+        <v>174.7088369382055</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -500,6 +533,15 @@
       <c r="H4">
         <v>239.640870302916</v>
       </c>
+      <c r="I4">
+        <v>1.562262044210526</v>
+      </c>
+      <c r="J4">
+        <v>27.821574</v>
+      </c>
+      <c r="K4">
+        <v>50.45070953745601</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,6 +576,15 @@
       <c r="H5">
         <v>2936.63346922398</v>
       </c>
+      <c r="I5">
+        <v>5.752896305810527</v>
+      </c>
+      <c r="J5">
+        <v>173.221967911579</v>
+      </c>
+      <c r="K5">
+        <v>618.2386250997853</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -568,6 +619,15 @@
       <c r="H6">
         <v>3571.11430312693</v>
       </c>
+      <c r="I6">
+        <v>11.67503847427368</v>
+      </c>
+      <c r="J6">
+        <v>271.6701719621053</v>
+      </c>
+      <c r="K6">
+        <v>751.8135375004063</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -602,6 +662,15 @@
       <c r="H7">
         <v>1357.16249629855</v>
       </c>
+      <c r="I7">
+        <v>6.607306417263158</v>
+      </c>
+      <c r="J7">
+        <v>105.9854692442105</v>
+      </c>
+      <c r="K7">
+        <v>285.7184202733789</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -636,6 +705,15 @@
       <c r="H8">
         <v>642.693928077817</v>
       </c>
+      <c r="I8">
+        <v>1.851242374568421</v>
+      </c>
+      <c r="J8">
+        <v>47.61016046736842</v>
+      </c>
+      <c r="K8">
+        <v>135.3039848584878</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -670,6 +748,15 @@
       <c r="H9">
         <v>47.7842741012573</v>
       </c>
+      <c r="I9">
+        <v>0.0772554332631579</v>
+      </c>
+      <c r="J9">
+        <v>2.772195305263158</v>
+      </c>
+      <c r="K9">
+        <v>10.05984717921207</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -704,6 +791,15 @@
       <c r="H10">
         <v>3911.74443353713</v>
       </c>
+      <c r="I10">
+        <v>8.512024420568421</v>
+      </c>
+      <c r="J10">
+        <v>232.7372274442105</v>
+      </c>
+      <c r="K10">
+        <v>823.5251439025537</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -738,6 +834,15 @@
       <c r="H11">
         <v>1396.59297868609</v>
       </c>
+      <c r="I11">
+        <v>2.250405597810526</v>
+      </c>
+      <c r="J11">
+        <v>77.66196274105265</v>
+      </c>
+      <c r="K11">
+        <v>294.0195744602295</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -772,6 +877,15 @@
       <c r="H12">
         <v>363.10868562758</v>
       </c>
+      <c r="I12">
+        <v>2.783947938947369</v>
+      </c>
+      <c r="J12">
+        <v>44.86441652631579</v>
+      </c>
+      <c r="K12">
+        <v>76.44393381633263</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -806,6 +920,15 @@
       <c r="H13">
         <v>1975.37827983499</v>
       </c>
+      <c r="I13">
+        <v>3.992151330736843</v>
+      </c>
+      <c r="J13">
+        <v>122.4105693473684</v>
+      </c>
+      <c r="K13">
+        <v>415.8691115442085</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -840,6 +963,15 @@
       <c r="H14">
         <v>1663.93286052346</v>
       </c>
+      <c r="I14">
+        <v>3.806496220042106</v>
+      </c>
+      <c r="J14">
+        <v>105.0628006357895</v>
+      </c>
+      <c r="K14">
+        <v>350.3016548470442</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -874,6 +1006,15 @@
       <c r="H15">
         <v>2845.98495420814</v>
       </c>
+      <c r="I15">
+        <v>9.330511474842107</v>
+      </c>
+      <c r="J15">
+        <v>205.9186638736842</v>
+      </c>
+      <c r="K15">
+        <v>599.1547272017137</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -908,6 +1049,15 @@
       <c r="H16">
         <v>1093.89645287395</v>
       </c>
+      <c r="I16">
+        <v>4.929034110736843</v>
+      </c>
+      <c r="J16">
+        <v>98.13871478105264</v>
+      </c>
+      <c r="K16">
+        <v>230.2939900787263</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -942,6 +1092,15 @@
       <c r="H17">
         <v>216.102864027023</v>
       </c>
+      <c r="I17">
+        <v>0.4750815332631579</v>
+      </c>
+      <c r="J17">
+        <v>13.91260854736842</v>
+      </c>
+      <c r="K17">
+        <v>45.49533979516274</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -976,6 +1135,15 @@
       <c r="H18">
         <v>293.948076710105</v>
       </c>
+      <c r="I18">
+        <v>0.1721581297052632</v>
+      </c>
+      <c r="J18">
+        <v>10.4894115031579</v>
+      </c>
+      <c r="K18">
+        <v>61.88380562318</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1010,6 +1178,15 @@
       <c r="H19">
         <v>1939.47662207484</v>
       </c>
+      <c r="I19">
+        <v>2.778527349705263</v>
+      </c>
+      <c r="J19">
+        <v>100.7358611452632</v>
+      </c>
+      <c r="K19">
+        <v>408.3108678052295</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1044,6 +1221,15 @@
       <c r="H20">
         <v>637.549638926983</v>
       </c>
+      <c r="I20">
+        <v>3.979530952842106</v>
+      </c>
+      <c r="J20">
+        <v>63.6915404</v>
+      </c>
+      <c r="K20">
+        <v>134.2209766162069</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1078,6 +1264,15 @@
       <c r="H21">
         <v>580.075658231974</v>
       </c>
+      <c r="I21">
+        <v>3.136567203557895</v>
+      </c>
+      <c r="J21">
+        <v>53.16588870736842</v>
+      </c>
+      <c r="K21">
+        <v>122.1211912067314</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1112,6 +1307,15 @@
       <c r="H22">
         <v>1438.98992925882</v>
       </c>
+      <c r="I22">
+        <v>41.97080872463158</v>
+      </c>
+      <c r="J22">
+        <v>813.5353737621053</v>
+      </c>
+      <c r="K22">
+        <v>302.9452482650148</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1146,6 +1350,15 @@
       <c r="H23">
         <v>3080.67969334126</v>
       </c>
+      <c r="I23">
+        <v>8.880253050399999</v>
+      </c>
+      <c r="J23">
+        <v>214.4468619978947</v>
+      </c>
+      <c r="K23">
+        <v>648.5641459665811</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1180,6 +1393,15 @@
       <c r="H24">
         <v>156.956790670753</v>
       </c>
+      <c r="I24">
+        <v>0.4057329838947369</v>
+      </c>
+      <c r="J24">
+        <v>11.71143556631579</v>
+      </c>
+      <c r="K24">
+        <v>33.04353487805327</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1214,6 +1436,15 @@
       <c r="H25">
         <v>2172.78481376171</v>
       </c>
+      <c r="I25">
+        <v>6.629473574336842</v>
+      </c>
+      <c r="J25">
+        <v>160.1976830568421</v>
+      </c>
+      <c r="K25">
+        <v>457.4283818445706</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1248,6 +1479,15 @@
       <c r="H26">
         <v>2043.97689397633</v>
       </c>
+      <c r="I26">
+        <v>4.940999035810527</v>
+      </c>
+      <c r="J26">
+        <v>131.2179087852632</v>
+      </c>
+      <c r="K26">
+        <v>430.3109250476484</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1282,6 +1522,15 @@
       <c r="H27">
         <v>60.6965613663197</v>
       </c>
+      <c r="I27">
+        <v>0.0820815800631579</v>
+      </c>
+      <c r="J27">
+        <v>3.014797389473685</v>
+      </c>
+      <c r="K27">
+        <v>12.77822344554099</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1316,6 +1565,15 @@
       <c r="H28">
         <v>4131.62300653756</v>
       </c>
+      <c r="I28">
+        <v>13.6762864016</v>
+      </c>
+      <c r="J28">
+        <v>296.9892338905264</v>
+      </c>
+      <c r="K28">
+        <v>869.8153697973811</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1350,6 +1608,15 @@
       <c r="H29">
         <v>202.082407623529</v>
       </c>
+      <c r="I29">
+        <v>0.5804620310947368</v>
+      </c>
+      <c r="J29">
+        <v>15.69426858947369</v>
+      </c>
+      <c r="K29">
+        <v>42.54366476284822</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1384,6 +1651,15 @@
       <c r="H30">
         <v>587.74931076169</v>
       </c>
+      <c r="I30">
+        <v>1.249397937789474</v>
+      </c>
+      <c r="J30">
+        <v>36.89789842526316</v>
+      </c>
+      <c r="K30">
+        <v>123.7366970024611</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1418,6 +1694,15 @@
       <c r="H31">
         <v>5285.25400102139</v>
       </c>
+      <c r="I31">
+        <v>17.68310916126316</v>
+      </c>
+      <c r="J31">
+        <v>374.0538568463158</v>
+      </c>
+      <c r="K31">
+        <v>1112.685052846608</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1452,6 +1737,15 @@
       <c r="H32">
         <v>2049.07706314325</v>
       </c>
+      <c r="I32">
+        <v>5.924979701410527</v>
+      </c>
+      <c r="J32">
+        <v>141.4486845915789</v>
+      </c>
+      <c r="K32">
+        <v>431.3846448722632</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1486,6 +1780,15 @@
       <c r="H33">
         <v>1495.45234002173</v>
       </c>
+      <c r="I33">
+        <v>1.795074395557895</v>
+      </c>
+      <c r="J33">
+        <v>72.64749219789475</v>
+      </c>
+      <c r="K33">
+        <v>314.8320715835221</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1520,6 +1823,15 @@
       <c r="H34">
         <v>1006.59189459682</v>
       </c>
+      <c r="I34">
+        <v>5.002326765010526</v>
+      </c>
+      <c r="J34">
+        <v>92.29313824210526</v>
+      </c>
+      <c r="K34">
+        <v>211.9140830730148</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1554,6 +1866,15 @@
       <c r="H35">
         <v>1123.45822021365</v>
       </c>
+      <c r="I35">
+        <v>1.689553236168421</v>
+      </c>
+      <c r="J35">
+        <v>62.12887537473684</v>
+      </c>
+      <c r="K35">
+        <v>236.517520044979</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1588,6 +1909,15 @@
       <c r="H36">
         <v>2774.26303608716</v>
       </c>
+      <c r="I36">
+        <v>7.7714278752</v>
+      </c>
+      <c r="J36">
+        <v>195.2661606168421</v>
+      </c>
+      <c r="K36">
+        <v>584.0553760183495</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1622,6 +1952,15 @@
       <c r="H37">
         <v>493.833147168159</v>
       </c>
+      <c r="I37">
+        <v>1.132436801431579</v>
+      </c>
+      <c r="J37">
+        <v>30.74581768842105</v>
+      </c>
+      <c r="K37">
+        <v>103.9648730880335</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1656,6 +1995,15 @@
       <c r="H38">
         <v>360.190888822079</v>
       </c>
+      <c r="I38">
+        <v>3.144676924210526</v>
+      </c>
+      <c r="J38">
+        <v>44.62719343157895</v>
+      </c>
+      <c r="K38">
+        <v>75.8296608046482</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1690,6 +2038,15 @@
       <c r="H39">
         <v>3981.38750062883</v>
       </c>
+      <c r="I39">
+        <v>5.615950019452632</v>
+      </c>
+      <c r="J39">
+        <v>200.7984088926316</v>
+      </c>
+      <c r="K39">
+        <v>838.1868422376484</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1724,6 +2081,15 @@
       <c r="H40">
         <v>90.7945650815964</v>
       </c>
+      <c r="I40">
+        <v>0.0943959037894737</v>
+      </c>
+      <c r="J40">
+        <v>4.316365296842105</v>
+      </c>
+      <c r="K40">
+        <v>19.11464528033609</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1758,6 +2124,15 @@
       <c r="H41">
         <v>4720.45389080048</v>
       </c>
+      <c r="I41">
+        <v>14.25753490730527</v>
+      </c>
+      <c r="J41">
+        <v>341.5704234147369</v>
+      </c>
+      <c r="K41">
+        <v>993.7797664843116</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1792,6 +2167,15 @@
       <c r="H42">
         <v>100.52829836309</v>
       </c>
+      <c r="I42">
+        <v>0.1888151355789474</v>
+      </c>
+      <c r="J42">
+        <v>6.09950347368421</v>
+      </c>
+      <c r="K42">
+        <v>21.16385228696632</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1826,6 +2210,15 @@
       <c r="H43">
         <v>3127.62896195054</v>
       </c>
+      <c r="I43">
+        <v>11.20361781107368</v>
+      </c>
+      <c r="J43">
+        <v>237.6274601705264</v>
+      </c>
+      <c r="K43">
+        <v>658.4482025159032</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1860,6 +2253,15 @@
       <c r="H44">
         <v>2907.24176007509</v>
       </c>
+      <c r="I44">
+        <v>13.51410746023158</v>
+      </c>
+      <c r="J44">
+        <v>248.0874200357895</v>
+      </c>
+      <c r="K44">
+        <v>612.0508968579137</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1894,6 +2296,15 @@
       <c r="H45">
         <v>265.037250190973</v>
       </c>
+      <c r="I45">
+        <v>0.5037157278526316</v>
+      </c>
+      <c r="J45">
+        <v>15.99710743789474</v>
+      </c>
+      <c r="K45">
+        <v>55.79731582967852</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1928,6 +2339,15 @@
       <c r="H46">
         <v>2533.31263515353</v>
       </c>
+      <c r="I46">
+        <v>12.12277348534737</v>
+      </c>
+      <c r="J46">
+        <v>220.8480723789474</v>
+      </c>
+      <c r="K46">
+        <v>533.3289758217959</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1962,6 +2382,15 @@
       <c r="H47">
         <v>1464.46751010418</v>
       </c>
+      <c r="I47">
+        <v>9.055624116273684</v>
+      </c>
+      <c r="J47">
+        <v>152.8199717115789</v>
+      </c>
+      <c r="K47">
+        <v>308.3089494956169</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1996,6 +2425,15 @@
       <c r="H48">
         <v>5341.57039743662</v>
       </c>
+      <c r="I48">
+        <v>30.29351157722105</v>
+      </c>
+      <c r="J48">
+        <v>491.3103162021054</v>
+      </c>
+      <c r="K48">
+        <v>1124.541136302446</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2030,6 +2468,15 @@
       <c r="H49">
         <v>4715.7360675782</v>
       </c>
+      <c r="I49">
+        <v>20.37434490126316</v>
+      </c>
+      <c r="J49">
+        <v>401.3414785557894</v>
+      </c>
+      <c r="K49">
+        <v>992.786540542779</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2064,6 +2511,15 @@
       <c r="H50">
         <v>497.00852894783</v>
       </c>
+      <c r="I50">
+        <v>4.82348638168421</v>
+      </c>
+      <c r="J50">
+        <v>63.76337402736842</v>
+      </c>
+      <c r="K50">
+        <v>104.6333745153326</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2098,6 +2554,15 @@
       <c r="H51">
         <v>2883.35612747073</v>
       </c>
+      <c r="I51">
+        <v>7.742804067894737</v>
+      </c>
+      <c r="J51">
+        <v>182.6601630294737</v>
+      </c>
+      <c r="K51">
+        <v>607.0223426254169</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2132,6 +2597,15 @@
       <c r="H52">
         <v>1320.29184257984</v>
       </c>
+      <c r="I52">
+        <v>8.635327050947369</v>
+      </c>
+      <c r="J52">
+        <v>135.1595720842105</v>
+      </c>
+      <c r="K52">
+        <v>277.9561773852295</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2166,6 +2640,15 @@
       <c r="H53">
         <v>737.95461127162</v>
       </c>
+      <c r="I53">
+        <v>2.513687818610527</v>
+      </c>
+      <c r="J53">
+        <v>58.20957232000001</v>
+      </c>
+      <c r="K53">
+        <v>155.3588655308674</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2200,6 +2683,15 @@
       <c r="H54">
         <v>93.468857884407</v>
       </c>
+      <c r="I54">
+        <v>0.2530292231578947</v>
+      </c>
+      <c r="J54">
+        <v>7.16639985263158</v>
+      </c>
+      <c r="K54">
+        <v>19.6776542914541</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2234,6 +2726,15 @@
       <c r="H55">
         <v>2659.6609596014</v>
       </c>
+      <c r="I55">
+        <v>8.274742979347369</v>
+      </c>
+      <c r="J55">
+        <v>197.4098309536842</v>
+      </c>
+      <c r="K55">
+        <v>559.928623073979</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2268,6 +2769,15 @@
       <c r="H56">
         <v>1498.83367209136</v>
       </c>
+      <c r="I56">
+        <v>8.038019140547368</v>
+      </c>
+      <c r="J56">
+        <v>121.8251180842105</v>
+      </c>
+      <c r="K56">
+        <v>315.5439309666021</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2302,6 +2812,15 @@
       <c r="H57">
         <v>85.1035608053207</v>
       </c>
+      <c r="I57">
+        <v>0.2404416813052632</v>
+      </c>
+      <c r="J57">
+        <v>6.165991376842105</v>
+      </c>
+      <c r="K57">
+        <v>17.91653911690962</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2336,6 +2855,15 @@
       <c r="H58">
         <v>2043.51015153527</v>
       </c>
+      <c r="I58">
+        <v>7.929277931410527</v>
+      </c>
+      <c r="J58">
+        <v>155.56640052</v>
+      </c>
+      <c r="K58">
+        <v>430.2126634811095</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2370,6 +2898,15 @@
       <c r="H59">
         <v>1757.07621058822</v>
       </c>
+      <c r="I59">
+        <v>9.757019166842106</v>
+      </c>
+      <c r="J59">
+        <v>156.1926092168421</v>
+      </c>
+      <c r="K59">
+        <v>369.9107811764674</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2404,6 +2941,15 @@
       <c r="H60">
         <v>777.641296386719</v>
       </c>
+      <c r="I60">
+        <v>3.936741540842105</v>
+      </c>
+      <c r="J60">
+        <v>70.87160134736843</v>
+      </c>
+      <c r="K60">
+        <v>163.7139571340461</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2438,6 +2984,15 @@
       <c r="H61">
         <v>189.457931756973</v>
       </c>
+      <c r="I61">
+        <v>0.7133730454736842</v>
+      </c>
+      <c r="J61">
+        <v>14.29178170526316</v>
+      </c>
+      <c r="K61">
+        <v>39.88588036988906</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2472,6 +3027,15 @@
       <c r="H62">
         <v>726.454589366913</v>
       </c>
+      <c r="I62">
+        <v>1.41964876391579</v>
+      </c>
+      <c r="J62">
+        <v>43.40385137894737</v>
+      </c>
+      <c r="K62">
+        <v>152.9378082877712</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2506,6 +3070,15 @@
       <c r="H63">
         <v>129.4337053895</v>
       </c>
+      <c r="I63">
+        <v>0.1057637154105263</v>
+      </c>
+      <c r="J63">
+        <v>5.490039389473685</v>
+      </c>
+      <c r="K63">
+        <v>27.24920113463158</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2540,6 +3113,15 @@
       <c r="H64">
         <v>172.813111960888</v>
       </c>
+      <c r="I64">
+        <v>0.8872403569052632</v>
+      </c>
+      <c r="J64">
+        <v>14.33355017684211</v>
+      </c>
+      <c r="K64">
+        <v>36.38170778123958</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2574,6 +3156,15 @@
       <c r="H65">
         <v>6647.77750423551</v>
       </c>
+      <c r="I65">
+        <v>21.1900275507579</v>
+      </c>
+      <c r="J65">
+        <v>501.8937786757895</v>
+      </c>
+      <c r="K65">
+        <v>1399.532106154844</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2608,6 +3199,15 @@
       <c r="H66">
         <v>704.042362749577</v>
       </c>
+      <c r="I66">
+        <v>1.742178649621053</v>
+      </c>
+      <c r="J66">
+        <v>47.05859093263158</v>
+      </c>
+      <c r="K66">
+        <v>148.2194447893846</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2642,6 +3242,15 @@
       <c r="H67">
         <v>2457.53724086285</v>
       </c>
+      <c r="I67">
+        <v>4.349893612063158</v>
+      </c>
+      <c r="J67">
+        <v>128.4074496484211</v>
+      </c>
+      <c r="K67">
+        <v>517.3762612342842</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2676,6 +3285,15 @@
       <c r="H68">
         <v>437.724057137966</v>
       </c>
+      <c r="I68">
+        <v>0.8005415714947368</v>
+      </c>
+      <c r="J68">
+        <v>27.47606235789474</v>
+      </c>
+      <c r="K68">
+        <v>92.15243308167706</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2710,6 +3328,15 @@
       <c r="H69">
         <v>5256.7250957787</v>
       </c>
+      <c r="I69">
+        <v>9.62625407608421</v>
+      </c>
+      <c r="J69">
+        <v>284.2093687284211</v>
+      </c>
+      <c r="K69">
+        <v>1106.678967532358</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2744,6 +3371,15 @@
       <c r="H70">
         <v>1151.78122808039</v>
       </c>
+      <c r="I70">
+        <v>5.695058900863159</v>
+      </c>
+      <c r="J70">
+        <v>99.76306308000001</v>
+      </c>
+      <c r="K70">
+        <v>242.48025854324</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2778,6 +3414,15 @@
       <c r="H71">
         <v>2850.50166559219</v>
       </c>
+      <c r="I71">
+        <v>8.245802120042105</v>
+      </c>
+      <c r="J71">
+        <v>205.6706167494737</v>
+      </c>
+      <c r="K71">
+        <v>600.1056138088821</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2812,6 +3457,15 @@
       <c r="H72">
         <v>3283.62657234073</v>
       </c>
+      <c r="I72">
+        <v>6.809133246463158</v>
+      </c>
+      <c r="J72">
+        <v>200.0881587852632</v>
+      </c>
+      <c r="K72">
+        <v>691.2898047033117</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2846,6 +3500,15 @@
       <c r="H73">
         <v>73.30098748207089</v>
       </c>
+      <c r="I73">
+        <v>0.03644744568421052</v>
+      </c>
+      <c r="J73">
+        <v>2.507745473684211</v>
+      </c>
+      <c r="K73">
+        <v>15.43178683833072</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2880,6 +3543,15 @@
       <c r="H74">
         <v>679.490454182029</v>
       </c>
+      <c r="I74">
+        <v>2.098398883305263</v>
+      </c>
+      <c r="J74">
+        <v>48.90367909473685</v>
+      </c>
+      <c r="K74">
+        <v>143.0506219330588</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2914,6 +3586,15 @@
       <c r="H75">
         <v>1885.02252429724</v>
       </c>
+      <c r="I75">
+        <v>6.999835473494738</v>
+      </c>
+      <c r="J75">
+        <v>148.8189250178947</v>
+      </c>
+      <c r="K75">
+        <v>396.8468472204716</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2948,6 +3629,15 @@
       <c r="H76">
         <v>561.9587989300491</v>
       </c>
+      <c r="I76">
+        <v>0.8649201792421053</v>
+      </c>
+      <c r="J76">
+        <v>30.1573063831579</v>
+      </c>
+      <c r="K76">
+        <v>118.3071155642209</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2982,6 +3672,15 @@
       <c r="H77">
         <v>469.772513896227</v>
       </c>
+      <c r="I77">
+        <v>0.6683261344631578</v>
+      </c>
+      <c r="J77">
+        <v>23.41219891578948</v>
+      </c>
+      <c r="K77">
+        <v>98.89947660973201</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3016,6 +3715,15 @@
       <c r="H78">
         <v>718.094665214419</v>
       </c>
+      <c r="I78">
+        <v>5.014210312610526</v>
+      </c>
+      <c r="J78">
+        <v>81.08222981263158</v>
+      </c>
+      <c r="K78">
+        <v>151.1778242556672</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3050,6 +3758,15 @@
       <c r="H79">
         <v>44.5000551342964</v>
       </c>
+      <c r="I79">
+        <v>0.1670177877894737</v>
+      </c>
+      <c r="J79">
+        <v>3.639772665263158</v>
+      </c>
+      <c r="K79">
+        <v>9.368432659851875</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3084,6 +3801,15 @@
       <c r="H80">
         <v>1230.26506608725</v>
       </c>
+      <c r="I80">
+        <v>3.59248640551579</v>
+      </c>
+      <c r="J80">
+        <v>82.72394422105263</v>
+      </c>
+      <c r="K80">
+        <v>259.0031718078421</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3118,6 +3844,15 @@
       <c r="H81">
         <v>69.8890905380249</v>
       </c>
+      <c r="I81">
+        <v>0.09289377221052632</v>
+      </c>
+      <c r="J81">
+        <v>3.745794610526316</v>
+      </c>
+      <c r="K81">
+        <v>14.71349274484735</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3152,6 +3887,15 @@
       <c r="H82">
         <v>4783.15413713455</v>
       </c>
+      <c r="I82">
+        <v>9.428220093663159</v>
+      </c>
+      <c r="J82">
+        <v>271.3619122042106</v>
+      </c>
+      <c r="K82">
+        <v>1006.979818344116</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3186,6 +3930,15 @@
       <c r="H83">
         <v>62.3581247329712</v>
       </c>
+      <c r="I83">
+        <v>0.05224266751578948</v>
+      </c>
+      <c r="J83">
+        <v>2.6207136</v>
+      </c>
+      <c r="K83">
+        <v>13.12802625957288</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3220,6 +3973,15 @@
       <c r="H84">
         <v>1610.4438637495</v>
       </c>
+      <c r="I84">
+        <v>4.016557388842106</v>
+      </c>
+      <c r="J84">
+        <v>110.9764958</v>
+      </c>
+      <c r="K84">
+        <v>339.0408134209474</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3254,6 +4016,15 @@
       <c r="H85">
         <v>1415.86216974258</v>
       </c>
+      <c r="I85">
+        <v>9.682739168294738</v>
+      </c>
+      <c r="J85">
+        <v>152.0783927684211</v>
+      </c>
+      <c r="K85">
+        <v>298.0762462615958</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3288,6 +4059,15 @@
       <c r="H86">
         <v>7221.39312213659</v>
       </c>
+      <c r="I86">
+        <v>20.99666467593684</v>
+      </c>
+      <c r="J86">
+        <v>471.145275088421</v>
+      </c>
+      <c r="K86">
+        <v>1520.293288870861</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3322,6 +4102,15 @@
       <c r="H87">
         <v>119.80144238472</v>
       </c>
+      <c r="I87">
+        <v>0.2181575654736842</v>
+      </c>
+      <c r="J87">
+        <v>7.293577073684211</v>
+      </c>
+      <c r="K87">
+        <v>25.22135629152</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3356,6 +4145,15 @@
       <c r="H88">
         <v>1871.32342034578</v>
       </c>
+      <c r="I88">
+        <v>13.85327046677895</v>
+      </c>
+      <c r="J88">
+        <v>188.2852029431579</v>
+      </c>
+      <c r="K88">
+        <v>393.9628253359537</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3390,6 +4188,15 @@
       <c r="H89">
         <v>753.966084957123</v>
       </c>
+      <c r="I89">
+        <v>7.968175117473685</v>
+      </c>
+      <c r="J89">
+        <v>93.93524611578947</v>
+      </c>
+      <c r="K89">
+        <v>158.7297020962364</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3424,6 +4231,15 @@
       <c r="H90">
         <v>232.220117777586</v>
       </c>
+      <c r="I90">
+        <v>0.7193046817473684</v>
+      </c>
+      <c r="J90">
+        <v>17.65671052421053</v>
+      </c>
+      <c r="K90">
+        <v>48.88844584791285</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3458,6 +4274,15 @@
       <c r="H91">
         <v>5980.54628427327</v>
       </c>
+      <c r="I91">
+        <v>13.93364633317895</v>
+      </c>
+      <c r="J91">
+        <v>374.1862120778948</v>
+      </c>
+      <c r="K91">
+        <v>1259.062375636478</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3492,6 +4317,15 @@
       <c r="H92">
         <v>321.63929527998</v>
       </c>
+      <c r="I92">
+        <v>1.134766763157895</v>
+      </c>
+      <c r="J92">
+        <v>26.06135654526316</v>
+      </c>
+      <c r="K92">
+        <v>67.71353584841684</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3526,6 +4360,15 @@
       <c r="H93">
         <v>591.678754836321</v>
       </c>
+      <c r="I93">
+        <v>1.308078343768421</v>
+      </c>
+      <c r="J93">
+        <v>36.11916761473685</v>
+      </c>
+      <c r="K93">
+        <v>124.5639483865939</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3560,6 +4403,15 @@
       <c r="H94">
         <v>98.576893299818</v>
       </c>
+      <c r="I94">
+        <v>0.09020908587368422</v>
+      </c>
+      <c r="J94">
+        <v>4.1051394</v>
+      </c>
+      <c r="K94">
+        <v>20.75303016838274</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3594,6 +4446,15 @@
       <c r="H95">
         <v>1103.26559726894</v>
       </c>
+      <c r="I95">
+        <v>5.264475506863159</v>
+      </c>
+      <c r="J95">
+        <v>99.17801966947368</v>
+      </c>
+      <c r="K95">
+        <v>232.2664415303032</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3628,6 +4489,15 @@
       <c r="H96">
         <v>8153.40737622976</v>
       </c>
+      <c r="I96">
+        <v>30.36282555263158</v>
+      </c>
+      <c r="J96">
+        <v>621.6411191494738</v>
+      </c>
+      <c r="K96">
+        <v>1716.506816048371</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3662,6 +4532,15 @@
       <c r="H97">
         <v>3501.78131073713</v>
       </c>
+      <c r="I97">
+        <v>12.88253045031579</v>
+      </c>
+      <c r="J97">
+        <v>267.5948738252632</v>
+      </c>
+      <c r="K97">
+        <v>737.2171180499221</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3696,6 +4575,15 @@
       <c r="H98">
         <v>3015.20736896992</v>
       </c>
+      <c r="I98">
+        <v>14.96619859282105</v>
+      </c>
+      <c r="J98">
+        <v>261.8041352084211</v>
+      </c>
+      <c r="K98">
+        <v>634.7804987305095</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3730,6 +4618,15 @@
       <c r="H99">
         <v>3250.74577653408</v>
       </c>
+      <c r="I99">
+        <v>12.02450421141053</v>
+      </c>
+      <c r="J99">
+        <v>241.7294593726316</v>
+      </c>
+      <c r="K99">
+        <v>684.3675319019117</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3764,6 +4661,15 @@
       <c r="H100">
         <v>878.908962816</v>
       </c>
+      <c r="I100">
+        <v>4.626789128736842</v>
+      </c>
+      <c r="J100">
+        <v>87.34220524842105</v>
+      </c>
+      <c r="K100">
+        <v>185.033465856</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3798,6 +4704,15 @@
       <c r="H101">
         <v>632.965787187219</v>
       </c>
+      <c r="I101">
+        <v>2.147408123642105</v>
+      </c>
+      <c r="J101">
+        <v>51.51578067368421</v>
+      </c>
+      <c r="K101">
+        <v>133.2559551973093</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3832,6 +4747,15 @@
       <c r="H102">
         <v>119.508729994297</v>
       </c>
+      <c r="I102">
+        <v>0.2060661842105263</v>
+      </c>
+      <c r="J102">
+        <v>6.485216147368422</v>
+      </c>
+      <c r="K102">
+        <v>25.15973263037832</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3866,6 +4790,15 @@
       <c r="H103">
         <v>251.476857274771</v>
       </c>
+      <c r="I103">
+        <v>0.4711741945263158</v>
+      </c>
+      <c r="J103">
+        <v>14.77503666105263</v>
+      </c>
+      <c r="K103">
+        <v>52.94249626837284</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3900,6 +4833,15 @@
       <c r="H104">
         <v>7072.52802658081</v>
       </c>
+      <c r="I104">
+        <v>15.47260104410526</v>
+      </c>
+      <c r="J104">
+        <v>418.9335160021053</v>
+      </c>
+      <c r="K104">
+        <v>1488.953268753855</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3934,6 +4876,15 @@
       <c r="H105">
         <v>514.384766757488</v>
       </c>
+      <c r="I105">
+        <v>0.9249343302947369</v>
+      </c>
+      <c r="J105">
+        <v>30.66852345052632</v>
+      </c>
+      <c r="K105">
+        <v>108.2915298436817</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3968,6 +4919,15 @@
       <c r="H106">
         <v>4388.75413790345</v>
       </c>
+      <c r="I106">
+        <v>8.7751457692</v>
+      </c>
+      <c r="J106">
+        <v>258.9721726147369</v>
+      </c>
+      <c r="K106">
+        <v>923.9482395586211</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4002,6 +4962,15 @@
       <c r="H107">
         <v>943.515495836735</v>
       </c>
+      <c r="I107">
+        <v>3.76348712631579</v>
+      </c>
+      <c r="J107">
+        <v>76.06409038736842</v>
+      </c>
+      <c r="K107">
+        <v>198.6348412287863</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4036,6 +5005,15 @@
       <c r="H108">
         <v>420.570912539959</v>
       </c>
+      <c r="I108">
+        <v>0.9896879685684211</v>
+      </c>
+      <c r="J108">
+        <v>28.79099055157895</v>
+      </c>
+      <c r="K108">
+        <v>88.54124474525453</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4070,6 +5048,15 @@
       <c r="H109">
         <v>3494.52579241991</v>
       </c>
+      <c r="I109">
+        <v>4.592793083536842</v>
+      </c>
+      <c r="J109">
+        <v>171.5568738568421</v>
+      </c>
+      <c r="K109">
+        <v>735.6896405094548</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4103,6 +5090,15 @@
       </c>
       <c r="H110">
         <v>321.864012271166</v>
+      </c>
+      <c r="I110">
+        <v>0.9233930372631579</v>
+      </c>
+      <c r="J110">
+        <v>22.14693414105263</v>
+      </c>
+      <c r="K110">
+        <v>67.76084468866654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>